<commit_message>
Embibe :: Updated Deeper logins
</commit_message>
<xml_diff>
--- a/EmbibeMobileApp/test-data/DeeperLogins.xlsx
+++ b/EmbibeMobileApp/test-data/DeeperLogins.xlsx
@@ -14470,7 +14470,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -14493,11 +14493,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -14529,22 +14544,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14841,205 +14859,202 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A101" sqref="A16:XFD101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" style="15" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="15" collapsed="1"/>
+    <col min="1" max="1" width="11.5703125" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.7109375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.28515625" style="12" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="12" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="15" t="s">
         <v>577</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="17" t="s">
         <v>380</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="15" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="18" customFormat="1">
-      <c r="A2" s="16" t="s">
-        <v>575</v>
-      </c>
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="1:4" s="14" customFormat="1">
+      <c r="A2" s="18" t="s">
+        <v>575</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>587</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D2" s="17"/>
-    </row>
-    <row r="3" spans="1:4" s="18" customFormat="1">
-      <c r="A3" s="16" t="s">
-        <v>576</v>
-      </c>
-      <c r="B3" s="16" t="s">
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" s="14" customFormat="1">
+      <c r="A3" s="18" t="s">
+        <v>576</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>615</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4" spans="1:4" s="18" customFormat="1">
-      <c r="A4" s="16" t="s">
-        <v>575</v>
-      </c>
-      <c r="B4" s="16" t="s">
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="1:4" s="14" customFormat="1">
+      <c r="A4" s="18" t="s">
+        <v>575</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>591</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:4" s="18" customFormat="1">
-      <c r="A5" s="16" t="s">
-        <v>576</v>
-      </c>
-      <c r="B5" s="16" t="s">
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:4" s="14" customFormat="1">
+      <c r="A5" s="18" t="s">
+        <v>576</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>579</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D5" s="17"/>
-    </row>
-    <row r="6" spans="1:4" s="18" customFormat="1">
-      <c r="A6" s="16" t="s">
-        <v>575</v>
-      </c>
-      <c r="B6" s="16" t="s">
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:4" s="14" customFormat="1">
+      <c r="A6" s="18" t="s">
+        <v>575</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>593</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D6" s="17"/>
-    </row>
-    <row r="7" spans="1:4" s="18" customFormat="1">
-      <c r="A7" s="16" t="s">
-        <v>576</v>
-      </c>
-      <c r="B7" s="16" t="s">
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:4" s="14" customFormat="1">
+      <c r="A7" s="18" t="s">
+        <v>576</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>586</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D7" s="17"/>
-    </row>
-    <row r="8" spans="1:4" s="18" customFormat="1">
-      <c r="A8" s="16" t="s">
-        <v>575</v>
-      </c>
-      <c r="B8" s="16" t="s">
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:4" s="14" customFormat="1">
+      <c r="A8" s="18" t="s">
+        <v>575</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>594</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D8" s="17"/>
-    </row>
-    <row r="9" spans="1:4" s="18" customFormat="1">
-      <c r="A9" s="16" t="s">
-        <v>576</v>
-      </c>
-      <c r="B9" s="16" t="s">
+      <c r="D8" s="19"/>
+    </row>
+    <row r="9" spans="1:4" s="14" customFormat="1">
+      <c r="A9" s="18" t="s">
+        <v>576</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>640</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D9" s="17"/>
-    </row>
-    <row r="10" spans="1:4" s="18" customFormat="1">
-      <c r="A10" s="16" t="s">
-        <v>575</v>
-      </c>
-      <c r="B10" s="16" t="s">
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:4" s="14" customFormat="1">
+      <c r="A10" s="18" t="s">
+        <v>575</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>589</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D10" s="17"/>
-    </row>
-    <row r="11" spans="1:4" s="18" customFormat="1">
-      <c r="A11" s="16" t="s">
-        <v>576</v>
-      </c>
-      <c r="B11" s="16" t="s">
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:4" s="14" customFormat="1">
+      <c r="A11" s="18" t="s">
+        <v>576</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>604</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D11" s="17"/>
-    </row>
-    <row r="12" spans="1:4" s="18" customFormat="1">
-      <c r="A12" s="16" t="s">
-        <v>576</v>
-      </c>
-      <c r="B12" s="16" t="s">
+      <c r="D11" s="19"/>
+    </row>
+    <row r="12" spans="1:4" s="14" customFormat="1">
+      <c r="A12" s="18" t="s">
+        <v>576</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>608</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D12" s="17"/>
-    </row>
-    <row r="13" spans="1:4" s="18" customFormat="1">
-      <c r="A13" s="16" t="s">
-        <v>575</v>
-      </c>
-      <c r="B13" s="16" t="s">
+      <c r="D12" s="19"/>
+    </row>
+    <row r="13" spans="1:4" s="14" customFormat="1">
+      <c r="A13" s="18" t="s">
+        <v>575</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>607</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D13" s="17"/>
-    </row>
-    <row r="14" spans="1:4" s="18" customFormat="1">
-      <c r="A14" s="16" t="s">
-        <v>575</v>
-      </c>
-      <c r="B14" s="16" t="s">
+      <c r="D13" s="19"/>
+    </row>
+    <row r="14" spans="1:4" s="14" customFormat="1">
+      <c r="A14" s="18" t="s">
+        <v>575</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>608</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D14" s="17"/>
-    </row>
-    <row r="15" spans="1:4" s="18" customFormat="1">
-      <c r="A15" s="16" t="s">
-        <v>576</v>
-      </c>
-      <c r="B15" s="16" t="s">
+      <c r="D14" s="19"/>
+    </row>
+    <row r="15" spans="1:4" s="14" customFormat="1">
+      <c r="A15" s="18" t="s">
+        <v>576</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>607</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="18" t="s">
         <v>4792</v>
       </c>
-      <c r="D15" s="17"/>
+      <c r="D15" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D15">
-    <filterColumn colId="0"/>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -60036,24 +60051,24 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="16" t="s">
-        <v>576</v>
-      </c>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="13" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>615</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>4792</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="16" t="s">
-        <v>576</v>
-      </c>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="13" t="s">
+        <v>576</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>579</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>4792</v>
       </c>
     </row>

</xml_diff>